<commit_message>
slight fix to write excel+retrieve_helper moved
</commit_message>
<xml_diff>
--- a/example_files/example.xlsx
+++ b/example_files/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\domilanza2002\repos\PlasFlowSolver\example_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32374E5-88E8-431B-A3D3-EF09B284178C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F42E986-23EA-47AC-8E60-E3D23CEF3178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t>Case=9</t>
   </si>
   <si>
-    <t>air</t>
-  </si>
-  <si>
     <t>Case=1</t>
   </si>
   <si>
@@ -169,13 +166,16 @@
     <t>CO2</t>
   </si>
   <si>
-    <t>db_example</t>
-  </si>
-  <si>
     <t>homann</t>
   </si>
   <si>
     <t>carleton</t>
+  </si>
+  <si>
+    <t>air_11</t>
+  </si>
+  <si>
+    <t>db_example.h5</t>
   </si>
 </sst>
 </file>
@@ -389,6 +389,9 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -432,9 +435,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -782,43 +782,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="30" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="33" t="s">
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="34"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="37"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="38"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
@@ -914,7 +914,7 @@
     </row>
     <row r="3" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="20">
         <v>1</v>
@@ -927,10 +927,10 @@
         <v>8.6</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -963,7 +963,7 @@
       <c r="T3" s="22">
         <v>100</v>
       </c>
-      <c r="U3" s="38">
+      <c r="U3" s="23">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V3" s="19" t="s">
@@ -975,13 +975,13 @@
       <c r="X3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y3" s="38">
+      <c r="Y3" s="23">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="Z3" s="22">
         <v>30</v>
       </c>
-      <c r="AA3" s="38">
+      <c r="AA3" s="23">
         <v>1E-4</v>
       </c>
       <c r="AB3" s="22">
@@ -993,7 +993,7 @@
     </row>
     <row r="4" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="20">
         <v>1</v>
@@ -1006,10 +1006,10 @@
         <v>34.46</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -1034,7 +1034,7 @@
         <v>35</v>
       </c>
       <c r="R4" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S4" s="22">
         <v>500</v>
@@ -1042,7 +1042,7 @@
       <c r="T4" s="22">
         <v>100</v>
       </c>
-      <c r="U4" s="38">
+      <c r="U4" s="23">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V4" s="19" t="s">
@@ -1054,13 +1054,13 @@
       <c r="X4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y4" s="38">
+      <c r="Y4" s="23">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="Z4" s="22">
         <v>30</v>
       </c>
-      <c r="AA4" s="38">
+      <c r="AA4" s="23">
         <v>1E-4</v>
       </c>
       <c r="AB4" s="22">
@@ -1072,7 +1072,7 @@
     </row>
     <row r="5" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="20">
         <v>1</v>
@@ -1085,10 +1085,10 @@
         <v>60.33</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -1113,7 +1113,7 @@
         <v>35</v>
       </c>
       <c r="R5" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S5" s="22">
         <v>500</v>
@@ -1121,7 +1121,7 @@
       <c r="T5" s="22">
         <v>100</v>
       </c>
-      <c r="U5" s="38">
+      <c r="U5" s="23">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V5" s="19" t="s">
@@ -1133,13 +1133,13 @@
       <c r="X5" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="38">
+      <c r="Y5" s="23">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="Z5" s="22">
         <v>30</v>
       </c>
-      <c r="AA5" s="38">
+      <c r="AA5" s="23">
         <v>1E-4</v>
       </c>
       <c r="AB5" s="22">
@@ -1151,7 +1151,7 @@
     </row>
     <row r="6" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="20">
         <v>1</v>
@@ -1164,7 +1164,7 @@
         <v>86.19</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>33</v>
@@ -1192,7 +1192,7 @@
         <v>35</v>
       </c>
       <c r="R6" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S6" s="22">
         <v>500</v>
@@ -1200,7 +1200,7 @@
       <c r="T6" s="22">
         <v>100</v>
       </c>
-      <c r="U6" s="38">
+      <c r="U6" s="23">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V6" s="19" t="s">
@@ -1212,13 +1212,13 @@
       <c r="X6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y6" s="38">
+      <c r="Y6" s="23">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="Z6" s="22">
         <v>30</v>
       </c>
-      <c r="AA6" s="38">
+      <c r="AA6" s="23">
         <v>1E-4</v>
       </c>
       <c r="AB6" s="22">
@@ -1230,7 +1230,7 @@
     </row>
     <row r="7" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="20">
         <v>1</v>
@@ -1243,7 +1243,7 @@
         <v>112.1</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="20">
@@ -1277,7 +1277,7 @@
         <v>35</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="S7" s="22">
         <v>500</v>
@@ -1285,7 +1285,7 @@
       <c r="T7" s="22">
         <v>100</v>
       </c>
-      <c r="U7" s="38">
+      <c r="U7" s="23">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V7" s="19" t="s">
@@ -1297,13 +1297,13 @@
       <c r="X7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y7" s="38">
+      <c r="Y7" s="23">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="Z7" s="22">
         <v>30</v>
       </c>
-      <c r="AA7" s="38">
+      <c r="AA7" s="23">
         <v>1E-4</v>
       </c>
       <c r="AB7" s="22">
@@ -1315,7 +1315,7 @@
     </row>
     <row r="8" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="20">
         <v>4</v>
@@ -1328,10 +1328,10 @@
         <v>137.9</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
@@ -1364,7 +1364,7 @@
       <c r="T8" s="22">
         <v>100</v>
       </c>
-      <c r="U8" s="38">
+      <c r="U8" s="23">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V8" s="19" t="s">
@@ -1376,13 +1376,13 @@
       <c r="X8" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y8" s="38">
+      <c r="Y8" s="23">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="Z8" s="22">
         <v>30</v>
       </c>
-      <c r="AA8" s="38">
+      <c r="AA8" s="23">
         <v>1E-4</v>
       </c>
       <c r="AB8" s="22">
@@ -1394,7 +1394,7 @@
     </row>
     <row r="9" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="20">
         <v>1</v>
@@ -1407,7 +1407,7 @@
         <v>163.80000000000001</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="20">
@@ -1441,7 +1441,7 @@
         <v>35</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="S9" s="22">
         <v>500</v>
@@ -1449,7 +1449,7 @@
       <c r="T9" s="22">
         <v>100</v>
       </c>
-      <c r="U9" s="38">
+      <c r="U9" s="23">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V9" s="19" t="s">
@@ -1461,13 +1461,13 @@
       <c r="X9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y9" s="38">
+      <c r="Y9" s="23">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="Z9" s="22">
         <v>30</v>
       </c>
-      <c r="AA9" s="38">
+      <c r="AA9" s="23">
         <v>1E-4</v>
       </c>
       <c r="AB9" s="22">
@@ -1479,7 +1479,7 @@
     </row>
     <row r="10" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="20">
         <v>2</v>
@@ -1492,7 +1492,7 @@
         <v>189.6</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="20">
@@ -1534,7 +1534,7 @@
       <c r="T10" s="22">
         <v>100</v>
       </c>
-      <c r="U10" s="38">
+      <c r="U10" s="23">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V10" s="19" t="s">
@@ -1546,13 +1546,13 @@
       <c r="X10" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y10" s="38">
+      <c r="Y10" s="23">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="Z10" s="22">
         <v>30</v>
       </c>
-      <c r="AA10" s="38">
+      <c r="AA10" s="23">
         <v>1E-4</v>
       </c>
       <c r="AB10" s="22">
@@ -1579,10 +1579,10 @@
         <v>34.46</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
@@ -1615,7 +1615,7 @@
       <c r="T11" s="22">
         <v>100</v>
       </c>
-      <c r="U11" s="38">
+      <c r="U11" s="23">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="V11" s="19" t="s">
@@ -1627,13 +1627,13 @@
       <c r="X11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y11" s="38">
+      <c r="Y11" s="23">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="Z11" s="22">
         <v>30</v>
       </c>
-      <c r="AA11" s="38">
+      <c r="AA11" s="23">
         <v>1E-4</v>
       </c>
       <c r="AB11" s="22">

</xml_diff>